<commit_message>
Update for water deficit calculation
equation digitized
</commit_message>
<xml_diff>
--- a/Weather_for_Penman/Irrigation_log.xlsx
+++ b/Weather_for_Penman/Irrigation_log.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DK/Documents/GitHub/SoilMoisture_analysis/Weather_for_Penman/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AA0216-7AEB-3F4B-A040-1667D54B68B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134890E2-1F81-E147-B153-3F0CE4F39E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="17480" windowWidth="26840" windowHeight="15940" xr2:uid="{AFA2ACD8-0CD5-2043-8D59-0A81AC23736D}"/>
+    <workbookView xWindow="2300" yWindow="4840" windowWidth="25560" windowHeight="18180" activeTab="1" xr2:uid="{AFA2ACD8-0CD5-2043-8D59-0A81AC23736D}"/>
   </bookViews>
   <sheets>
     <sheet name="irrigation_log" sheetId="1" r:id="rId1"/>
+    <sheet name="deficit_adj" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,15 +37,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Corn(hr)</t>
-  </si>
-  <si>
-    <t>Soybean(hr)</t>
+    <t>Corn IRR (hr)</t>
+  </si>
+  <si>
+    <t>Corn FERT (hr)</t>
+  </si>
+  <si>
+    <t>Soybean IRR (hr)</t>
+  </si>
+  <si>
+    <t>Soybean FERT (hr)</t>
+  </si>
+  <si>
+    <t>Corn IRR (inch)</t>
+  </si>
+  <si>
+    <t>Soybean IRR (inch)</t>
+  </si>
+  <si>
+    <t>Corn FERT (inch)</t>
+  </si>
+  <si>
+    <t>Soybean FERT (inch)</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -417,15 +439,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF4E0D44-5547-8E42-9336-7F1CCC28BE18}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,10 +455,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>45397</v>
       </c>
@@ -444,153 +472,393 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>45398</v>
       </c>
       <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>45399</v>
       </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
       <c r="C4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>45400</v>
       </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
       <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>45401</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>45402</v>
       </c>
       <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
         <v>3</v>
       </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>45403</v>
       </c>
       <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>45404</v>
       </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
       <c r="C9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>45405</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>45406</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>45407</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>45408</v>
       </c>
       <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>45409</v>
       </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
       <c r="C14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>45410</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>45411</v>
       </c>
       <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>45412</v>
       </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
       <c r="C17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>45413</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>45414</v>
       </c>
       <c r="B19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>45415</v>
       </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
       <c r="C20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>45416</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69FDD65C-8F8C-F543-BD88-99EEF0A5725C}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>45413</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mesonet data update (mesonet)
updated to use mesonet data
(pending)
</commit_message>
<xml_diff>
--- a/Weather_for_Penman/Irrigation_log.xlsx
+++ b/Weather_for_Penman/Irrigation_log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DK/Documents/GitHub/SoilMoisture_analysis/Weather_for_Penman/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134890E2-1F81-E147-B153-3F0CE4F39E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC95AB27-5448-694B-BEAC-82CE1423C403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2300" yWindow="4840" windowWidth="25560" windowHeight="18180" activeTab="1" xr2:uid="{AFA2ACD8-0CD5-2043-8D59-0A81AC23736D}"/>
   </bookViews>
@@ -54,6 +54,9 @@
     <t>Soybean FERT (hr)</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>Corn IRR (inch)</t>
   </si>
   <si>
@@ -64,9 +67,6 @@
   </si>
   <si>
     <t>Soybean FERT (inch)</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
 </sst>
 </file>
@@ -814,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69FDD65C-8F8C-F543-BD88-99EEF0A5725C}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -832,16 +832,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -855,7 +855,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E2">
         <v>1</v>

</xml_diff>